<commit_message>
updated data and code
</commit_message>
<xml_diff>
--- a/config/config_group.xlsx
+++ b/config/config_group.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanghyun/github/pypsa_alternative/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE93C6A-9729-1A47-969E-ACA6C1BE1B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BE0B97-2CFD-7748-8E4A-547D3CC06FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22580" yWindow="8500" windowWidth="27700" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22580" yWindow="8500" windowWidth="27700" windowHeight="17540" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modelling_setting" sheetId="17" r:id="rId1"/>
@@ -1362,7 +1362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F667B4A-1409-A340-9A81-2DB2EB65E934}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2108,7 +2108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2198,7 +2198,7 @@
         <v>255</v>
       </c>
       <c r="B8" t="s">
-        <v>284</v>
+        <v>145</v>
       </c>
       <c r="C8" t="s">
         <v>146</v>

</xml_diff>